<commit_message>
wildcatSTK - Core : Seasonality decomposition for multiplicative models added + unit tests - Green
Signed-off-by: Orzobimbumbam <alberto.campi@aol.co.uk>
</commit_message>
<xml_diff>
--- a/UnitTests/JSONSerialiser/ExcelInputs/sample_dataSet_clean.xlsx
+++ b/UnitTests/JSONSerialiser/ExcelInputs/sample_dataSet_clean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="211">
   <si>
     <t>Date</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t>RPI_FOOD_DRINK_TOBACCO_NSA</t>
+  </si>
+  <si>
+    <t>OV_UK_VISITORS_NSA</t>
   </si>
 </sst>
 </file>
@@ -717,8 +720,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -728,9 +733,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1023,15 +1030,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L199"/>
+  <dimension ref="A1:M199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1080,11 @@
       <c r="L1" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1106,8 +1121,11 @@
       <c r="L2" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1144,8 +1162,11 @@
       <c r="L3" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1182,8 +1203,11 @@
       <c r="L4" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1220,8 +1244,11 @@
       <c r="L5" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1258,8 +1285,11 @@
       <c r="L6" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1296,8 +1326,11 @@
       <c r="L7" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1334,8 +1367,11 @@
       <c r="L8" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1372,8 +1408,11 @@
       <c r="L9" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1410,8 +1449,11 @@
       <c r="L10" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1448,8 +1490,11 @@
       <c r="L11" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1486,8 +1531,11 @@
       <c r="L12" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1524,8 +1572,11 @@
       <c r="L13" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1562,8 +1613,11 @@
       <c r="L14" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1600,8 +1654,11 @@
       <c r="L15" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1638,8 +1695,11 @@
       <c r="L16" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1676,8 +1736,11 @@
       <c r="L17" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1714,8 +1777,11 @@
       <c r="L18" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1752,8 +1818,11 @@
       <c r="L19" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1790,8 +1859,11 @@
       <c r="L20" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1828,8 +1900,11 @@
       <c r="L21" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1866,8 +1941,11 @@
       <c r="L22" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1904,8 +1982,11 @@
       <c r="L23" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1942,8 +2023,11 @@
       <c r="L24" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1980,8 +2064,11 @@
       <c r="L25" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2018,8 +2105,11 @@
       <c r="L26" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2056,8 +2146,11 @@
       <c r="L27" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2094,8 +2187,11 @@
       <c r="L28" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2132,8 +2228,11 @@
       <c r="L29" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2170,8 +2269,11 @@
       <c r="L30" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -2208,8 +2310,11 @@
       <c r="L31" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2246,8 +2351,11 @@
       <c r="L32" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2284,8 +2392,11 @@
       <c r="L33" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -2322,8 +2433,11 @@
       <c r="L34" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="M34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2360,8 +2474,11 @@
       <c r="L35" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="M35" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -2398,8 +2515,11 @@
       <c r="L36" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="M36" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -2436,8 +2556,11 @@
       <c r="L37" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="M37" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -2474,8 +2597,11 @@
       <c r="L38" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="M38" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -2512,8 +2638,11 @@
       <c r="L39" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="M39" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -2550,8 +2679,11 @@
       <c r="L40" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="M40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -2588,8 +2720,11 @@
       <c r="L41" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="M41" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2626,8 +2761,11 @@
       <c r="L42" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="M42">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -2664,8 +2802,11 @@
       <c r="L43" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="M43">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -2702,8 +2843,11 @@
       <c r="L44" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="M44">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -2740,8 +2884,11 @@
       <c r="L45" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -2778,8 +2925,11 @@
       <c r="L46" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -2816,8 +2966,11 @@
       <c r="L47" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="M47">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -2854,8 +3007,11 @@
       <c r="L48" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="49" spans="1:12">
+      <c r="M48">
+        <v>4261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -2892,8 +3048,11 @@
       <c r="L49" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="50" spans="1:12">
+      <c r="M49">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -2930,8 +3089,11 @@
       <c r="L50" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="51" spans="1:12">
+      <c r="M50">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -2968,8 +3130,11 @@
       <c r="L51" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="52" spans="1:12">
+      <c r="M51">
+        <v>3174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3006,8 +3171,11 @@
       <c r="L52" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="53" spans="1:12">
+      <c r="M52">
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3044,8 +3212,11 @@
       <c r="L53" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="54" spans="1:12">
+      <c r="M53">
+        <v>2196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -3082,8 +3253,11 @@
       <c r="L54" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="55" spans="1:12">
+      <c r="M54">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3120,8 +3294,11 @@
       <c r="L55" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="56" spans="1:12">
+      <c r="M55">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -3158,8 +3335,11 @@
       <c r="L56" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="M56">
+        <v>4714</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -3196,8 +3376,11 @@
       <c r="L57" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="M57">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -3234,8 +3417,11 @@
       <c r="L58" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="M58">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -3272,8 +3458,11 @@
       <c r="L59" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="M59">
+        <v>3582</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -3310,8 +3499,11 @@
       <c r="L60" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="M60">
+        <v>5180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -3348,8 +3540,11 @@
       <c r="L61" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="M61">
+        <v>2727</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -3386,8 +3581,11 @@
       <c r="L62" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="M62">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -3424,8 +3622,11 @@
       <c r="L63" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="M63">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -3462,8 +3663,11 @@
       <c r="L64" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="M64">
+        <v>5405</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -3500,8 +3704,11 @@
       <c r="L65" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="66" spans="1:12">
+      <c r="M65">
+        <v>2751</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -3538,8 +3745,11 @@
       <c r="L66" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="M66">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -3576,8 +3786,11 @@
       <c r="L67" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="68" spans="1:12">
+      <c r="M67">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -3614,8 +3827,11 @@
       <c r="L68" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="69" spans="1:12">
+      <c r="M68">
+        <v>5065</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -3652,8 +3868,11 @@
       <c r="L69" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="70" spans="1:12">
+      <c r="M69">
+        <v>2933</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -3690,8 +3909,11 @@
       <c r="L70" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="71" spans="1:12">
+      <c r="M70">
+        <v>2641</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -3728,8 +3950,11 @@
       <c r="L71" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="72" spans="1:12">
+      <c r="M71">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -3766,8 +3991,11 @@
       <c r="L72" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="73" spans="1:12">
+      <c r="M72">
+        <v>5618</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>82</v>
       </c>
@@ -3804,8 +4032,11 @@
       <c r="L73" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="74" spans="1:12">
+      <c r="M73">
+        <v>3259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>83</v>
       </c>
@@ -3842,8 +4073,11 @@
       <c r="L74" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="75" spans="1:12">
+      <c r="M74">
+        <v>2777</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -3880,8 +4114,11 @@
       <c r="L75" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="76" spans="1:12">
+      <c r="M75">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>85</v>
       </c>
@@ -3918,8 +4155,11 @@
       <c r="L76" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="77" spans="1:12">
+      <c r="M76">
+        <v>5549</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>86</v>
       </c>
@@ -3956,8 +4196,11 @@
       <c r="L77" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="M77">
+        <v>3460</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>87</v>
       </c>
@@ -3994,8 +4237,11 @@
       <c r="L78" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="79" spans="1:12">
+      <c r="M78">
+        <v>3337</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -4032,8 +4278,11 @@
       <c r="L79" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="80" spans="1:12">
+      <c r="M79">
+        <v>4265</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>89</v>
       </c>
@@ -4070,8 +4319,11 @@
       <c r="L80" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="81" spans="1:12">
+      <c r="M80">
+        <v>5961</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -4108,8 +4360,11 @@
       <c r="L81" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="82" spans="1:12">
+      <c r="M81">
+        <v>3776</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>91</v>
       </c>
@@ -4146,8 +4401,11 @@
       <c r="L82" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="83" spans="1:12">
+      <c r="M82">
+        <v>3323</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>92</v>
       </c>
@@ -4184,8 +4442,11 @@
       <c r="L83" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="84" spans="1:12">
+      <c r="M83">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>93</v>
       </c>
@@ -4222,8 +4483,11 @@
       <c r="L84" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="85" spans="1:12">
+      <c r="M84">
+        <v>6306</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -4260,8 +4524,11 @@
       <c r="L85" t="e">
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="86" spans="1:12">
+      <c r="M85">
+        <v>3851</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>95</v>
       </c>
@@ -4298,8 +4565,11 @@
       <c r="L86">
         <v>43.3</v>
       </c>
-    </row>
-    <row r="87" spans="1:12">
+      <c r="M86">
+        <v>2836</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>96</v>
       </c>
@@ -4336,8 +4606,11 @@
       <c r="L87">
         <v>46.2</v>
       </c>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="M87">
+        <v>4297</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" t="s">
         <v>97</v>
       </c>
@@ -4374,8 +4647,11 @@
       <c r="L88">
         <v>46.4</v>
       </c>
-    </row>
-    <row r="89" spans="1:12">
+      <c r="M88">
+        <v>6012</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>98</v>
       </c>
@@ -4412,8 +4688,11 @@
       <c r="L89">
         <v>49.5</v>
       </c>
-    </row>
-    <row r="90" spans="1:12">
+      <c r="M89">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>99</v>
       </c>
@@ -4450,8 +4729,11 @@
       <c r="L90">
         <v>46.4</v>
       </c>
-    </row>
-    <row r="91" spans="1:12">
+      <c r="M90">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>100</v>
       </c>
@@ -4488,8 +4770,11 @@
       <c r="L91">
         <v>48.8</v>
       </c>
-    </row>
-    <row r="92" spans="1:12">
+      <c r="M91">
+        <v>4897</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>101</v>
       </c>
@@ -4526,8 +4811,11 @@
       <c r="L92">
         <v>47.1</v>
       </c>
-    </row>
-    <row r="93" spans="1:12">
+      <c r="M92">
+        <v>6188</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -4564,8 +4852,11 @@
       <c r="L93">
         <v>51.4</v>
       </c>
-    </row>
-    <row r="94" spans="1:12">
+      <c r="M93">
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" t="s">
         <v>103</v>
       </c>
@@ -4602,8 +4893,11 @@
       <c r="L94">
         <v>48.1</v>
       </c>
-    </row>
-    <row r="95" spans="1:12">
+      <c r="M94">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>104</v>
       </c>
@@ -4640,8 +4934,11 @@
       <c r="L95">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="96" spans="1:12">
+      <c r="M95">
+        <v>5222</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" t="s">
         <v>105</v>
       </c>
@@ -4678,8 +4975,11 @@
       <c r="L96">
         <v>49.6</v>
       </c>
-    </row>
-    <row r="97" spans="1:12">
+      <c r="M96">
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" t="s">
         <v>106</v>
       </c>
@@ -4716,8 +5016,11 @@
       <c r="L97">
         <v>53.4</v>
       </c>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="M97">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -4754,8 +5057,11 @@
       <c r="L98">
         <v>49.7</v>
       </c>
-    </row>
-    <row r="99" spans="1:12">
+      <c r="M98">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" t="s">
         <v>108</v>
       </c>
@@ -4792,8 +5098,11 @@
       <c r="L99">
         <v>51.6</v>
       </c>
-    </row>
-    <row r="100" spans="1:12">
+      <c r="M99">
+        <v>5269</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" t="s">
         <v>109</v>
       </c>
@@ -4830,8 +5139,11 @@
       <c r="L100">
         <v>51.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:12">
+      <c r="M100">
+        <v>6891</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>110</v>
       </c>
@@ -4868,8 +5180,11 @@
       <c r="L101">
         <v>55.9</v>
       </c>
-    </row>
-    <row r="102" spans="1:12">
+      <c r="M101">
+        <v>4794</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" t="s">
         <v>111</v>
       </c>
@@ -4906,8 +5221,11 @@
       <c r="L102">
         <v>51.1</v>
       </c>
-    </row>
-    <row r="103" spans="1:12">
+      <c r="M102">
+        <v>4217</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
       <c r="A103" t="s">
         <v>112</v>
       </c>
@@ -4944,8 +5262,11 @@
       <c r="L103">
         <v>54.2</v>
       </c>
-    </row>
-    <row r="104" spans="1:12">
+      <c r="M103">
+        <v>5952</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
       <c r="A104" t="s">
         <v>113</v>
       </c>
@@ -4982,8 +5303,11 @@
       <c r="L104">
         <v>54</v>
       </c>
-    </row>
-    <row r="105" spans="1:12">
+      <c r="M104">
+        <v>7747</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" t="s">
         <v>114</v>
       </c>
@@ -5020,8 +5344,11 @@
       <c r="L105">
         <v>58.4</v>
       </c>
-    </row>
-    <row r="106" spans="1:12">
+      <c r="M105">
+        <v>5622</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -5058,8 +5385,11 @@
       <c r="L106">
         <v>54</v>
       </c>
-    </row>
-    <row r="107" spans="1:12">
+      <c r="M106">
+        <v>4719</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -5096,8 +5426,11 @@
       <c r="L107">
         <v>56.9</v>
       </c>
-    </row>
-    <row r="108" spans="1:12">
+      <c r="M107">
+        <v>6680</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -5134,8 +5467,11 @@
       <c r="L108">
         <v>56.2</v>
       </c>
-    </row>
-    <row r="109" spans="1:12">
+      <c r="M108">
+        <v>8130</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -5172,8 +5508,11 @@
       <c r="L109">
         <v>59.9</v>
       </c>
-    </row>
-    <row r="110" spans="1:12">
+      <c r="M109">
+        <v>5631</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -5210,8 +5549,11 @@
       <c r="L110">
         <v>55.8</v>
       </c>
-    </row>
-    <row r="111" spans="1:12">
+      <c r="M110">
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -5248,8 +5590,11 @@
       <c r="L111">
         <v>57.7</v>
       </c>
-    </row>
-    <row r="112" spans="1:12">
+      <c r="M111">
+        <v>6446</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -5286,8 +5631,11 @@
       <c r="L112">
         <v>57.6</v>
       </c>
-    </row>
-    <row r="113" spans="1:12">
+      <c r="M112">
+        <v>8168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -5324,8 +5672,11 @@
       <c r="L113">
         <v>61.8</v>
       </c>
-    </row>
-    <row r="114" spans="1:12">
+      <c r="M113">
+        <v>5961</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -5362,8 +5713,11 @@
       <c r="L114">
         <v>57.3</v>
       </c>
-    </row>
-    <row r="115" spans="1:12">
+      <c r="M114">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -5400,8 +5754,11 @@
       <c r="L115">
         <v>60.3</v>
       </c>
-    </row>
-    <row r="116" spans="1:12">
+      <c r="M115">
+        <v>6834</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
       <c r="A116" t="s">
         <v>125</v>
       </c>
@@ -5438,8 +5795,11 @@
       <c r="L116">
         <v>58.6</v>
       </c>
-    </row>
-    <row r="117" spans="1:12">
+      <c r="M116">
+        <v>8028</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
       <c r="A117" t="s">
         <v>126</v>
       </c>
@@ -5476,8 +5836,11 @@
       <c r="L117">
         <v>63.6</v>
       </c>
-    </row>
-    <row r="118" spans="1:12">
+      <c r="M117">
+        <v>6080</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
       <c r="A118" t="s">
         <v>127</v>
       </c>
@@ -5514,8 +5877,11 @@
       <c r="L118">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="119" spans="1:12">
+      <c r="M118">
+        <v>5046</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13">
       <c r="A119" t="s">
         <v>128</v>
       </c>
@@ -5552,8 +5918,11 @@
       <c r="L119">
         <v>60.7</v>
       </c>
-    </row>
-    <row r="120" spans="1:12">
+      <c r="M119">
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" t="s">
         <v>129</v>
       </c>
@@ -5590,8 +5959,11 @@
       <c r="L120">
         <v>59.3</v>
       </c>
-    </row>
-    <row r="121" spans="1:12">
+      <c r="M120">
+        <v>7912</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
       <c r="A121" t="s">
         <v>130</v>
       </c>
@@ -5628,8 +6000,11 @@
       <c r="L121">
         <v>65.400000000000006</v>
       </c>
-    </row>
-    <row r="122" spans="1:12">
+      <c r="M121">
+        <v>5636</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
       <c r="A122" t="s">
         <v>131</v>
       </c>
@@ -5666,8 +6041,11 @@
       <c r="L122">
         <v>59.7</v>
       </c>
-    </row>
-    <row r="123" spans="1:12">
+      <c r="M122">
+        <v>4993</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
       <c r="A123" t="s">
         <v>132</v>
       </c>
@@ -5704,8 +6082,11 @@
       <c r="L123">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="124" spans="1:12">
+      <c r="M123">
+        <v>6733</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13">
       <c r="A124" t="s">
         <v>133</v>
       </c>
@@ -5742,8 +6123,11 @@
       <c r="L124">
         <v>61.5</v>
       </c>
-    </row>
-    <row r="125" spans="1:12">
+      <c r="M124">
+        <v>7943</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
       <c r="A125" t="s">
         <v>134</v>
       </c>
@@ -5780,8 +6164,11 @@
       <c r="L125">
         <v>67.7</v>
       </c>
-    </row>
-    <row r="126" spans="1:12">
+      <c r="M125">
+        <v>5538</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
       <c r="A126" t="s">
         <v>135</v>
       </c>
@@ -5818,8 +6205,11 @@
       <c r="L126">
         <v>61.7</v>
       </c>
-    </row>
-    <row r="127" spans="1:12">
+      <c r="M126">
+        <v>4862</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
       <c r="A127" t="s">
         <v>136</v>
       </c>
@@ -5856,8 +6246,11 @@
       <c r="L127">
         <v>66</v>
       </c>
-    </row>
-    <row r="128" spans="1:12">
+      <c r="M127">
+        <v>6279</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -5894,8 +6287,11 @@
       <c r="L128">
         <v>64.8</v>
       </c>
-    </row>
-    <row r="129" spans="1:12">
+      <c r="M128">
+        <v>7098</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
       <c r="A129" t="s">
         <v>138</v>
       </c>
@@ -5932,8 +6328,11 @@
       <c r="L129">
         <v>71.2</v>
       </c>
-    </row>
-    <row r="130" spans="1:12">
+      <c r="M129">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
       <c r="A130" t="s">
         <v>139</v>
       </c>
@@ -5970,8 +6369,11 @@
       <c r="L130">
         <v>65.3</v>
       </c>
-    </row>
-    <row r="131" spans="1:12">
+      <c r="M130">
+        <v>4558</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
       <c r="A131" t="s">
         <v>140</v>
       </c>
@@ -6008,8 +6410,11 @@
       <c r="L131">
         <v>67.599999999999994</v>
       </c>
-    </row>
-    <row r="132" spans="1:12">
+      <c r="M131">
+        <v>6509</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
       <c r="A132" t="s">
         <v>141</v>
       </c>
@@ -6046,8 +6451,11 @@
       <c r="L132">
         <v>66.8</v>
       </c>
-    </row>
-    <row r="133" spans="1:12">
+      <c r="M132">
+        <v>7619</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
       <c r="A133" t="s">
         <v>142</v>
       </c>
@@ -6084,8 +6492,11 @@
       <c r="L133">
         <v>72.7</v>
       </c>
-    </row>
-    <row r="134" spans="1:12">
+      <c r="M133">
+        <v>5706</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
       <c r="A134" t="s">
         <v>143</v>
       </c>
@@ -6122,8 +6533,11 @@
       <c r="L134">
         <v>66.8</v>
       </c>
-    </row>
-    <row r="135" spans="1:12">
+      <c r="M134">
+        <v>4926</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
       <c r="A135" t="s">
         <v>144</v>
       </c>
@@ -6160,8 +6574,11 @@
       <c r="L135">
         <v>70.099999999999994</v>
       </c>
-    </row>
-    <row r="136" spans="1:12">
+      <c r="M135">
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
       <c r="A136" t="s">
         <v>145</v>
       </c>
@@ -6198,8 +6615,11 @@
       <c r="L136">
         <v>69.3</v>
       </c>
-    </row>
-    <row r="137" spans="1:12">
+      <c r="M136">
+        <v>7716</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
       <c r="A137" t="s">
         <v>146</v>
       </c>
@@ -6236,8 +6656,11 @@
       <c r="L137">
         <v>74.7</v>
       </c>
-    </row>
-    <row r="138" spans="1:12">
+      <c r="M137">
+        <v>6147</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
       <c r="A138" t="s">
         <v>147</v>
       </c>
@@ -6274,8 +6697,11 @@
       <c r="L138">
         <v>69.099999999999994</v>
       </c>
-    </row>
-    <row r="139" spans="1:12">
+      <c r="M138">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
       <c r="A139" t="s">
         <v>148</v>
       </c>
@@ -6312,8 +6738,11 @@
       <c r="L139">
         <v>72.400000000000006</v>
       </c>
-    </row>
-    <row r="140" spans="1:12">
+      <c r="M139">
+        <v>7015</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
       <c r="A140" t="s">
         <v>149</v>
       </c>
@@ -6350,8 +6779,11 @@
       <c r="L140">
         <v>72</v>
       </c>
-    </row>
-    <row r="141" spans="1:12">
+      <c r="M140">
+        <v>8412</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
       <c r="A141" t="s">
         <v>150</v>
       </c>
@@ -6388,8 +6820,11 @@
       <c r="L141">
         <v>77.900000000000006</v>
       </c>
-    </row>
-    <row r="142" spans="1:12">
+      <c r="M141">
+        <v>6748</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
       <c r="A142" t="s">
         <v>151</v>
       </c>
@@ -6426,8 +6861,11 @@
       <c r="L142">
         <v>71.400000000000006</v>
       </c>
-    </row>
-    <row r="143" spans="1:12">
+      <c r="M142">
+        <v>6171</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
       <c r="A143" t="s">
         <v>152</v>
       </c>
@@ -6464,8 +6902,11 @@
       <c r="L143">
         <v>74.5</v>
       </c>
-    </row>
-    <row r="144" spans="1:12">
+      <c r="M143">
+        <v>7868</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
       <c r="A144" t="s">
         <v>153</v>
       </c>
@@ -6502,8 +6943,11 @@
       <c r="L144">
         <v>73.400000000000006</v>
       </c>
-    </row>
-    <row r="145" spans="1:12">
+      <c r="M144">
+        <v>8858</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13">
       <c r="A145" t="s">
         <v>154</v>
       </c>
@@ -6540,8 +6984,11 @@
       <c r="L145">
         <v>80.099999999999994</v>
       </c>
-    </row>
-    <row r="146" spans="1:12">
+      <c r="M145">
+        <v>7073</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13">
       <c r="A146" t="s">
         <v>155</v>
       </c>
@@ -6578,8 +7025,11 @@
       <c r="L146">
         <v>71.900000000000006</v>
       </c>
-    </row>
-    <row r="147" spans="1:12">
+      <c r="M146">
+        <v>6351</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13">
       <c r="A147" t="s">
         <v>156</v>
       </c>
@@ -6616,8 +7066,11 @@
       <c r="L147">
         <v>77.2</v>
       </c>
-    </row>
-    <row r="148" spans="1:12">
+      <c r="M147">
+        <v>8476</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13">
       <c r="A148" t="s">
         <v>157</v>
       </c>
@@ -6654,8 +7107,11 @@
       <c r="L148">
         <v>77</v>
       </c>
-    </row>
-    <row r="149" spans="1:12">
+      <c r="M148">
+        <v>10296</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13">
       <c r="A149" t="s">
         <v>158</v>
       </c>
@@ -6692,8 +7148,11 @@
       <c r="L149">
         <v>83.8</v>
       </c>
-    </row>
-    <row r="150" spans="1:12">
+      <c r="M149">
+        <v>7592</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13">
       <c r="A150" t="s">
         <v>159</v>
       </c>
@@ -6730,8 +7189,11 @@
       <c r="L150">
         <v>75.900000000000006</v>
       </c>
-    </row>
-    <row r="151" spans="1:12">
+      <c r="M150">
+        <v>6737</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13">
       <c r="A151" t="s">
         <v>160</v>
       </c>
@@ -6768,8 +7230,11 @@
       <c r="L151">
         <v>80.3</v>
       </c>
-    </row>
-    <row r="152" spans="1:12">
+      <c r="M151">
+        <v>8511</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13">
       <c r="A152" t="s">
         <v>161</v>
       </c>
@@ -6806,8 +7271,11 @@
       <c r="L152">
         <v>79</v>
       </c>
-    </row>
-    <row r="153" spans="1:12">
+      <c r="M152">
+        <v>9564</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13">
       <c r="A153" t="s">
         <v>162</v>
       </c>
@@ -6844,8 +7312,11 @@
       <c r="L153">
         <v>86.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:12">
+      <c r="M153">
+        <v>7966</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13">
       <c r="A154" t="s">
         <v>163</v>
       </c>
@@ -6882,8 +7353,11 @@
       <c r="L154">
         <v>80.400000000000006</v>
       </c>
-    </row>
-    <row r="155" spans="1:12">
+      <c r="M154">
+        <v>7195</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13">
       <c r="A155" t="s">
         <v>164</v>
       </c>
@@ -6920,8 +7394,11 @@
       <c r="L155">
         <v>85.3</v>
       </c>
-    </row>
-    <row r="156" spans="1:12">
+      <c r="M155">
+        <v>8406</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13">
       <c r="A156" t="s">
         <v>165</v>
       </c>
@@ -6958,8 +7435,11 @@
       <c r="L156">
         <v>84.4</v>
       </c>
-    </row>
-    <row r="157" spans="1:12">
+      <c r="M156">
+        <v>9358</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13">
       <c r="A157" t="s">
         <v>166</v>
       </c>
@@ -6996,8 +7476,11 @@
       <c r="L157">
         <v>91.2</v>
       </c>
-    </row>
-    <row r="158" spans="1:12">
+      <c r="M157">
+        <v>6929</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13">
       <c r="A158" t="s">
         <v>167</v>
       </c>
@@ -7034,8 +7517,11 @@
       <c r="L158">
         <v>85.3</v>
       </c>
-    </row>
-    <row r="159" spans="1:12">
+      <c r="M158">
+        <v>6213</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13">
       <c r="A159" t="s">
         <v>168</v>
       </c>
@@ -7072,8 +7558,11 @@
       <c r="L159">
         <v>90.3</v>
       </c>
-    </row>
-    <row r="160" spans="1:12">
+      <c r="M159">
+        <v>7943</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13">
       <c r="A160" t="s">
         <v>169</v>
       </c>
@@ -7110,8 +7599,11 @@
       <c r="L160">
         <v>87.8</v>
       </c>
-    </row>
-    <row r="161" spans="1:12">
+      <c r="M160">
+        <v>8779</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13">
       <c r="A161" t="s">
         <v>170</v>
       </c>
@@ -7148,8 +7640,11 @@
       <c r="L161">
         <v>93.4</v>
       </c>
-    </row>
-    <row r="162" spans="1:12">
+      <c r="M161">
+        <v>6951</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13">
       <c r="A162" t="s">
         <v>171</v>
       </c>
@@ -7186,8 +7681,11 @@
       <c r="L162">
         <v>86.6</v>
       </c>
-    </row>
-    <row r="163" spans="1:12">
+      <c r="M162">
+        <v>5904</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13">
       <c r="A163" t="s">
         <v>172</v>
       </c>
@@ -7224,8 +7722,11 @@
       <c r="L163">
         <v>90.9</v>
       </c>
-    </row>
-    <row r="164" spans="1:12">
+      <c r="M163">
+        <v>7755</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13">
       <c r="A164" t="s">
         <v>173</v>
       </c>
@@ -7262,8 +7763,11 @@
       <c r="L164">
         <v>88.4</v>
       </c>
-    </row>
-    <row r="165" spans="1:12">
+      <c r="M164">
+        <v>8985</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13">
       <c r="A165" t="s">
         <v>174</v>
       </c>
@@ -7300,8 +7804,11 @@
       <c r="L165">
         <v>94.9</v>
       </c>
-    </row>
-    <row r="166" spans="1:12">
+      <c r="M165">
+        <v>7160</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13">
       <c r="A166" t="s">
         <v>175</v>
       </c>
@@ -7338,8 +7845,11 @@
       <c r="L166">
         <v>87.7</v>
       </c>
-    </row>
-    <row r="167" spans="1:12">
+      <c r="M166">
+        <v>6113</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13">
       <c r="A167" t="s">
         <v>176</v>
       </c>
@@ -7376,8 +7886,11 @@
       <c r="L167">
         <v>94.1</v>
       </c>
-    </row>
-    <row r="168" spans="1:12">
+      <c r="M167">
+        <v>8308</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13">
       <c r="A168" t="s">
         <v>177</v>
       </c>
@@ -7414,8 +7927,11 @@
       <c r="L168">
         <v>92.7</v>
       </c>
-    </row>
-    <row r="169" spans="1:12">
+      <c r="M168">
+        <v>9172</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13">
       <c r="A169" t="s">
         <v>178</v>
       </c>
@@ -7452,8 +7968,11 @@
       <c r="L169">
         <v>100.2</v>
       </c>
-    </row>
-    <row r="170" spans="1:12">
+      <c r="M169">
+        <v>7205</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13">
       <c r="A170" t="s">
         <v>179</v>
       </c>
@@ -7490,8 +8009,11 @@
       <c r="L170">
         <v>91.7</v>
       </c>
-    </row>
-    <row r="171" spans="1:12">
+      <c r="M170">
+        <v>6249</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13">
       <c r="A171" t="s">
         <v>180</v>
       </c>
@@ -7528,8 +8050,11 @@
       <c r="L171">
         <v>96.5</v>
       </c>
-    </row>
-    <row r="172" spans="1:12">
+      <c r="M171">
+        <v>8457</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13">
       <c r="A172" t="s">
         <v>181</v>
       </c>
@@ -7566,8 +8091,11 @@
       <c r="L172">
         <v>95.3</v>
       </c>
-    </row>
-    <row r="173" spans="1:12">
+      <c r="M172">
+        <v>8786</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13">
       <c r="A173" t="s">
         <v>182</v>
       </c>
@@ -7604,8 +8132,11 @@
       <c r="L173">
         <v>102.3</v>
       </c>
-    </row>
-    <row r="174" spans="1:12">
+      <c r="M173">
+        <v>7593</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13">
       <c r="A174" t="s">
         <v>183</v>
       </c>
@@ -7642,8 +8173,11 @@
       <c r="L174">
         <v>94.9</v>
       </c>
-    </row>
-    <row r="175" spans="1:12">
+      <c r="M174">
+        <v>6332</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13">
       <c r="A175" t="s">
         <v>184</v>
       </c>
@@ -7680,8 +8214,11 @@
       <c r="L175">
         <v>98.5</v>
       </c>
-    </row>
-    <row r="176" spans="1:12">
+      <c r="M175">
+        <v>8869</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13">
       <c r="A176" t="s">
         <v>185</v>
       </c>
@@ -7718,8 +8255,11 @@
       <c r="L176">
         <v>99.3</v>
       </c>
-    </row>
-    <row r="177" spans="1:12">
+      <c r="M176">
+        <v>9645</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13">
       <c r="A177" t="s">
         <v>186</v>
       </c>
@@ -7756,8 +8296,11 @@
       <c r="L177">
         <v>106</v>
       </c>
-    </row>
-    <row r="178" spans="1:12">
+      <c r="M177">
+        <v>7843</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13">
       <c r="A178" t="s">
         <v>187</v>
       </c>
@@ -7794,8 +8337,11 @@
       <c r="L178">
         <v>95</v>
       </c>
-    </row>
-    <row r="179" spans="1:12">
+      <c r="M178">
+        <v>6810</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13">
       <c r="A179" t="s">
         <v>188</v>
       </c>
@@ -7832,8 +8378,11 @@
       <c r="L179">
         <v>98.8</v>
       </c>
-    </row>
-    <row r="180" spans="1:12">
+      <c r="M179">
+        <v>9490</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13">
       <c r="A180" t="s">
         <v>189</v>
       </c>
@@ -7870,8 +8419,11 @@
       <c r="L180">
         <v>95.6</v>
       </c>
-    </row>
-    <row r="181" spans="1:12">
+      <c r="M180">
+        <v>10030</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13">
       <c r="A181" t="s">
         <v>190</v>
       </c>
@@ -7908,8 +8460,11 @@
       <c r="L181">
         <v>102.7</v>
       </c>
-    </row>
-    <row r="182" spans="1:12">
+      <c r="M181">
+        <v>8050</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13">
       <c r="A182" t="s">
         <v>191</v>
       </c>
@@ -7946,8 +8501,11 @@
       <c r="L182">
         <v>95</v>
       </c>
-    </row>
-    <row r="183" spans="1:12">
+      <c r="M182">
+        <v>6949</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13">
       <c r="A183" t="s">
         <v>192</v>
       </c>
@@ -7984,8 +8542,11 @@
       <c r="L183">
         <v>97.6</v>
       </c>
-    </row>
-    <row r="184" spans="1:12">
+      <c r="M183">
+        <v>9983</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13">
       <c r="A184" t="s">
         <v>193</v>
       </c>
@@ -8022,8 +8583,11 @@
       <c r="L184">
         <v>95.7</v>
       </c>
-    </row>
-    <row r="185" spans="1:12">
+      <c r="M184">
+        <v>10499</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13">
       <c r="A185" t="s">
         <v>194</v>
       </c>
@@ -8060,8 +8624,11 @@
       <c r="L185">
         <v>102.9</v>
       </c>
-    </row>
-    <row r="186" spans="1:12">
+      <c r="M185">
+        <v>8683</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13">
       <c r="A186" t="s">
         <v>195</v>
       </c>
@@ -8098,8 +8665,11 @@
       <c r="L186">
         <v>95.4</v>
       </c>
-    </row>
-    <row r="187" spans="1:12">
+      <c r="M186">
+        <v>7551</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13">
       <c r="A187" t="s">
         <v>196</v>
       </c>
@@ -8136,8 +8706,11 @@
       <c r="L187">
         <v>99</v>
       </c>
-    </row>
-    <row r="188" spans="1:12">
+      <c r="M187">
+        <v>9968</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13">
       <c r="A188" t="s">
         <v>197</v>
       </c>
@@ -8174,8 +8747,11 @@
       <c r="L188">
         <v>98.7</v>
       </c>
-    </row>
-    <row r="189" spans="1:12">
+      <c r="M188">
+        <v>10659</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13">
       <c r="A189" t="s">
         <v>198</v>
       </c>
@@ -8212,8 +8788,11 @@
       <c r="L189">
         <v>107</v>
       </c>
-    </row>
-    <row r="190" spans="1:12">
+      <c r="M189">
+        <v>9432</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13">
       <c r="A190" t="s">
         <v>199</v>
       </c>
@@ -8250,8 +8829,11 @@
       <c r="L190">
         <v>96.7</v>
       </c>
-    </row>
-    <row r="191" spans="1:12">
+      <c r="M190">
+        <v>8307</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13">
       <c r="A191" t="s">
         <v>200</v>
       </c>
@@ -8288,8 +8870,11 @@
       <c r="L191">
         <v>103.1</v>
       </c>
-    </row>
-    <row r="192" spans="1:12">
+      <c r="M191">
+        <v>10877</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13">
       <c r="A192" t="s">
         <v>201</v>
       </c>
@@ -8326,8 +8911,11 @@
       <c r="L192">
         <v>100.8</v>
       </c>
-    </row>
-    <row r="193" spans="1:12">
+      <c r="M192">
+        <v>11110</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13">
       <c r="A193" t="s">
         <v>202</v>
       </c>
@@ -8364,8 +8952,11 @@
       <c r="L193">
         <v>111</v>
       </c>
-    </row>
-    <row r="194" spans="1:12">
+      <c r="M193">
+        <v>8920</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13">
       <c r="A194" t="s">
         <v>203</v>
       </c>
@@ -8402,8 +8993,11 @@
       <c r="L194">
         <v>100.9</v>
       </c>
-    </row>
-    <row r="195" spans="1:12">
+      <c r="M194">
+        <v>7883</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13">
       <c r="A195" t="s">
         <v>204</v>
       </c>
@@ -8440,8 +9034,11 @@
       <c r="L195">
         <v>106.2</v>
       </c>
-    </row>
-    <row r="196" spans="1:12">
+      <c r="M195">
+        <v>10056</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13">
       <c r="A196" t="s">
         <v>205</v>
       </c>
@@ -8478,8 +9075,11 @@
       <c r="L196">
         <v>107.7</v>
       </c>
-    </row>
-    <row r="197" spans="1:12">
+      <c r="M196">
+        <v>10802</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13">
       <c r="A197" t="s">
         <v>206</v>
       </c>
@@ -8516,8 +9116,11 @@
       <c r="L197">
         <v>116.4</v>
       </c>
-    </row>
-    <row r="198" spans="1:12">
+      <c r="M197">
+        <v>9163</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13">
       <c r="A198" t="s">
         <v>207</v>
       </c>
@@ -8554,8 +9157,11 @@
       <c r="L198">
         <v>106</v>
       </c>
-    </row>
-    <row r="199" spans="1:12">
+      <c r="M198">
+        <v>7956</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13">
       <c r="A199" t="s">
         <v>208</v>
       </c>
@@ -8591,6 +9197,9 @@
       </c>
       <c r="L199">
         <v>112.8</v>
+      </c>
+      <c r="M199">
+        <v>9593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>